<commit_message>
Finished V1.0 whisker module
</commit_message>
<xml_diff>
--- a/Documentation/BOM template.xlsx
+++ b/Documentation/BOM template.xlsx
@@ -496,7 +496,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H15" sqref="A2:H15"/>
+      <selection pane="bottomLeft" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,7 +903,10 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="7">
+        <f>SUM(Table3[Quantity])</f>
+        <v>0</v>
+      </c>
       <c r="K21" s="8">
         <f>SUM(Table3[Total])</f>
         <v>0</v>

</xml_diff>